<commit_message>
changing how I assing individual count and the columns for the template and conversion
</commit_message>
<xml_diff>
--- a/data/digitized_data/HJ-8-occ-entry-template_22-11-11.xlsx
+++ b/data/digitized_data/HJ-8-occ-entry-template_22-11-11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/digitized_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF51825-92CD-F142-9020-6973ECF8B29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C47B38-D490-734A-931D-7C2410B419E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15320" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
   </bookViews>
@@ -4030,8 +4030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E2B542-A597-DF4D-A726-D9C00BB4087B}">
   <dimension ref="A1:AH173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
@@ -4068,7 +4068,7 @@
     <col min="29" max="29" width="9.1640625" style="4" customWidth="1"/>
     <col min="30" max="30" width="14.6640625" style="4" customWidth="1"/>
     <col min="31" max="31" width="10.83203125" style="4"/>
-    <col min="32" max="32" width="14.33203125" style="4" customWidth="1"/>
+    <col min="32" max="32" width="17.33203125" style="4" customWidth="1"/>
     <col min="33" max="33" width="29.5" style="4" customWidth="1"/>
     <col min="34" max="34" width="70.6640625" style="4" customWidth="1"/>
     <col min="35" max="16384" width="10.83203125" style="4"/>

</xml_diff>